<commit_message>
2nd commit moving_animated.mp4 with some bugs
</commit_message>
<xml_diff>
--- a/script.xlsx
+++ b/script.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kang-wooyong/Desktop/work/auto-lecture-generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AAB417-8A1F-2942-8C72-F9F72796CA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192BA4B0-3273-C346-9D35-0283DDB05A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="5460" windowWidth="18680" windowHeight="17860" xr2:uid="{3EEF23B7-4254-A74E-957D-AC805A26204E}"/>
+    <workbookView xWindow="27900" yWindow="4640" windowWidth="18680" windowHeight="17860" xr2:uid="{3EEF23B7-4254-A74E-957D-AC805A26204E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,10 +46,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">안녕하세요. 인재개발부의 강우용 대리입니다. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>콘텐츠 제작 지원 신청 이용 가이드에 대해서 설명드리도록 하겠습니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -79,6 +75,10 @@
   </si>
   <si>
     <t xml:space="preserve">지금까지 콘텐츠 제작 지원 신청 가이드 설명이었습니다. 감사합니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">안녕하세요. 드래곤볼의 손오공입니다! </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -466,7 +466,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -487,7 +487,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -495,7 +495,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -503,7 +503,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -511,7 +511,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -519,7 +519,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -527,7 +527,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -535,7 +535,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -543,7 +543,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -551,7 +551,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>